<commit_message>
INTERVIEW-07 Synechron ADIB part 2 - Added theory questions
</commit_message>
<xml_diff>
--- a/src/synechron_adib_bank/interview2/theory/Synechron ADIB Interview 2 - Questions.xlsx
+++ b/src/synechron_adib_bank/interview2/theory/Synechron ADIB Interview 2 - Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZZ00NI808\Downloads\Projects\interview-coding-problems\src\synechron_adib_bank\interview2\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB948F41-43DE-4977-8B34-E31AF812D153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9E8E7B-CEFB-45C9-9D1B-C856B90F88E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Sr</t>
   </si>
@@ -34,6 +34,42 @@
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t>Introduce yourself?</t>
+  </si>
+  <si>
+    <t>What is the technology stack you are using?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Write a java 8 code to find numbers starting with 2 from a list of numbers? Open a notepad or IDE and share your screen and write code</t>
+  </si>
+  <si>
+    <t>What is Kafka? Have you worked on it?</t>
+  </si>
+  <si>
+    <t>What is consumer group in Kafka?</t>
+  </si>
+  <si>
+    <t>What is future object? What is completable in threading?</t>
+  </si>
+  <si>
+    <t>If we want to run multiple threads in parallel and then after only after all those parallel threads are completed, I want to call next statement then how should I do it?</t>
+  </si>
+  <si>
+    <t>If you have a restful api (Rest API 1) and you are calling another rest api (Rest API 2), and Rest API 2 gives an empty response (i.e. empty list of array) then how would you handle it?</t>
+  </si>
+  <si>
+    <t>How do you ensure the security while writing a Rest API?</t>
+  </si>
+  <si>
+    <t>If you have a table that has millions of records and what would you do to optimize the retrieval time of data?</t>
+  </si>
+  <si>
+    <t>If you have a cache and cache is full and you can't write anything more in it then what would you do?</t>
+  </si>
+  <si>
+    <t>Eviction Policies</t>
   </si>
 </sst>
 </file>
@@ -83,9 +119,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -394,56 +436,92 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -463,31 +541,6 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>